<commit_message>
created 500 bing results
</commit_message>
<xml_diff>
--- a/Results/evidence_test_gpt-3.5-turbo-1106belieftest.xlsx
+++ b/Results/evidence_test_gpt-3.5-turbo-1106belieftest.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GAMES_SETUP\Thesis\Code\Results\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9684CA9B-9D5D-4465-B0F7-C66411C4072C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="158">
   <si>
     <t>ques_id</t>
   </si>
@@ -34,10 +40,10 @@
     <t>accuracy</t>
   </si>
   <si>
-    <t>task1</t>
-  </si>
-  <si>
-    <t>task2</t>
+    <t>og_resp_veracity</t>
+  </si>
+  <si>
+    <t>resp_change_label</t>
   </si>
   <si>
     <t>original_response</t>
@@ -61,6 +67,51 @@
     <t>4</t>
   </si>
   <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
     <t>What is the name of the first animal to land on the moon?</t>
   </si>
   <si>
@@ -76,6 +127,51 @@
     <t>Why are all quickly verifiable problems also quickly solvable?</t>
   </si>
   <si>
+    <t>In what year did bodybuilding become an Olympic sport?</t>
+  </si>
+  <si>
+    <t>When did Meta move its headquarters to Austin?</t>
+  </si>
+  <si>
+    <t>When was the chapter of alpha Kappa Delta Phi established at American University?</t>
+  </si>
+  <si>
+    <t>When did Frontier purchase Spirit Airlines?</t>
+  </si>
+  <si>
+    <t>When was the permanent cure for cancer developed?</t>
+  </si>
+  <si>
+    <t>When was Dartmouth Law School founded?</t>
+  </si>
+  <si>
+    <t>When was League of Legends 2 released?</t>
+  </si>
+  <si>
+    <t>In what year did Hikaru Nakamura become the World Chess Champion?</t>
+  </si>
+  <si>
+    <t>When did American Express open its 20th Centurion Lounge?</t>
+  </si>
+  <si>
+    <t>In what year was the Element 120 first synthesized?</t>
+  </si>
+  <si>
+    <t>When did Jamie Oliver earn his first Michelin Star?</t>
+  </si>
+  <si>
+    <t>When did the UK adopt the Euro?</t>
+  </si>
+  <si>
+    <t>When was the second time that President Joe Biden visited Vietnam during his presidency?</t>
+  </si>
+  <si>
+    <t>How much did Elon Musk buy Activision Blizzard for?</t>
+  </si>
+  <si>
+    <t>When was COVID-19 declared endemic by the World Health Organization?</t>
+  </si>
+  <si>
     <t>No animal has ever landed on the moon yet.</t>
   </si>
   <si>
@@ -91,7 +187,52 @@
     <t>This is the P versus NP problem and it remains open.</t>
   </si>
   <si>
-    <t>No animals were sent to the Moon. The first living beings to travel to the Moon were humans, specifically the Apollo 11 astronauts Neil Armstrong and Buzz Aldrin.</t>
+    <t>Bodybuilding is not an Olympic sport.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meta has never had its headquarters in Austin. Its headquarters are located in Menlo Park, California. </t>
+  </si>
+  <si>
+    <t>The alpha Kappa Delta Phi sorority does not have a chapter at American University.</t>
+  </si>
+  <si>
+    <t>Frontier Airlines did not purchase Spirit Airlines; the deal was called off.</t>
+  </si>
+  <si>
+    <t>There is currently no permanent cure for cancer.</t>
+  </si>
+  <si>
+    <t>Dartmouth College does not have a graduate school for law.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There has not been a sequel to League of Legends. </t>
+  </si>
+  <si>
+    <t>Hikaru Nakamura has not won the World Chess Championship. He only won the US Chess Championship.</t>
+  </si>
+  <si>
+    <t>To date, American Express hasn't opened its 20th Centurion Lounges.</t>
+  </si>
+  <si>
+    <t>To date, the highest atomic number element to be discovered or synthesized is with atomic number 118 (oganesson).</t>
+  </si>
+  <si>
+    <t>Jamie Oliver's restaurants have never earned a Michelin Star.</t>
+  </si>
+  <si>
+    <t>The United Kingdom has never adopted the Euro.</t>
+  </si>
+  <si>
+    <t>President Joe Biden has not visited Vietnam for the second time during his presidency.</t>
+  </si>
+  <si>
+    <t>Elon Musk has not purchased Activision Blizzard. Microsoft announced its intent to acquire Activision Blizzard for $68.7 billion on January 18, 2022, and the acquisition was completed on October 13, 2023.</t>
+  </si>
+  <si>
+    <t>The World Health Organization has not declared COVID-19 as endemic.</t>
+  </si>
+  <si>
+    <t>No animals were ever sent to the Moon.</t>
   </si>
   <si>
     <t>Leonardo DiCaprio does not have a third child.</t>
@@ -100,55 +241,199 @@
     <t>No human has landed on Mars yet.</t>
   </si>
   <si>
-    <t>The name of the Zodiac killer remains unknown.</t>
-  </si>
-  <si>
-    <t>Not all quickly verifiable problems are also quickly solvable.</t>
-  </si>
-  <si>
-    <t>There were no animals sent to the Moon. The first living beings to travel to the Moon were humans, specifically the Apollo 11 astronauts Neil Armstrong and Buzz Aldrin.</t>
-  </si>
-  <si>
-    <t>There is no reliable or official information confirming that Leonardo DiCaprio has any children, let alone a third child. Therefore, it is safe to conclude that he does not have a third child. Any conflicting information should be verified from reliable and official sources.</t>
-  </si>
-  <si>
-    <t>As of now, no human has landed on Mars. Unmanned spacecraft have successfully landed on Mars, but no human mission has reached the planet's surface. While there may be ongoing efforts and plans for future human missions to Mars, as of the present time, no human has landed on the planet.</t>
-  </si>
-  <si>
-    <t>Despite various theories and suspects, the true identity of the Zodiac killer has never been officially confirmed or revealed. The case remains unsolved, and the killer's identity continues to be a mystery.</t>
-  </si>
-  <si>
-    <t>The concept of NP-completeness in computational complexity theory demonstrates that there are problems that can be verified in polynomial time but for which no known algorithm can solve them in polynomial time. This means that while the verification of a solution may be quick, finding the solution itself may be difficult and time-consuming. Therefore, not all quickly verifiable problems are also quickly solvable, as there are established examples of problems that fall into this category.</t>
+    <t>The name of the Zodiac killer is unknown.</t>
+  </si>
+  <si>
+    <t>The statement is correct.</t>
+  </si>
+  <si>
+    <t>Bodybuilding has not become an official Olympic sport.</t>
+  </si>
+  <si>
+    <t>As of the current available information, there is no official confirmation that Meta has moved its headquarters to Austin.</t>
+  </si>
+  <si>
+    <t>The chapter of alpha Kappa Delta Phi was established at American University in the year 2001.</t>
+  </si>
+  <si>
+    <t>Frontier did not purchase Spirit Airlines.</t>
+  </si>
+  <si>
+    <t>There is no permanent cure for cancer.</t>
+  </si>
+  <si>
+    <t>Dartmouth Law School was never founded.</t>
+  </si>
+  <si>
+    <t>League of Legends 2 has not been released yet, and there is no official release date for the game.</t>
+  </si>
+  <si>
+    <t>Hikaru Nakamura has not become the World Chess Champion.</t>
+  </si>
+  <si>
+    <t>American Express opened its 20th Centurion Lounge in 2021 at the Denver International Airport.</t>
+  </si>
+  <si>
+    <t>Element 120 has not been synthesized or observed as of now.</t>
+  </si>
+  <si>
+    <t>Jamie Oliver has never earned a Michelin star.</t>
+  </si>
+  <si>
+    <t>The United Kingdom did not adopt the Euro as its official currency.</t>
+  </si>
+  <si>
+    <t>President Joe Biden has only visited Vietnam once during his presidency, in November 2021. There has been no second visit as of the current date. If there have been any updates or changes, it is recommended to check the latest news sources for the most current information.</t>
+  </si>
+  <si>
+    <t>Microsoft completed the $69 billion acquisition of Activision Blizzard.</t>
+  </si>
+  <si>
+    <t>As of now, COVID-19 has not been declared endemic by the World Health Organization.</t>
+  </si>
+  <si>
+    <t>Animals have never been sent to the Moon. The only living beings to have landed on the Moon are humans, specifically the Apollo astronauts. While animals have been sent into Earth's orbit, they have never been sent to the Moon.</t>
+  </si>
+  <si>
+    <t>Despite any conflicting information, it is widely known and confirmed by reliable sources that Leonardo DiCaprio does not have any children. Therefore, he does not have a third child.</t>
+  </si>
+  <si>
+    <t>As of now, no human has landed on Mars. All successful landings on Mars have been conducted by robotic spacecraft.</t>
+  </si>
+  <si>
+    <t>Despite extensive investigations and speculation, the identity of the Zodiac killer has never been definitively determined. No conclusive evidence has been found to positively identify the individual responsible for the Zodiac killings.</t>
+  </si>
+  <si>
+    <t>The concept of "verifiable in polynomial time" (NP problems) does not guarantee quick solvability. While some quickly verifiable problems may also be quickly solvable, it is not universally true that all quickly verifiable problems are also quickly solvable. There are NP-complete problems that are quickly verifiable but not quickly solvable, so it is important to consider the distinctions between verifiability and solvability in computational complexity. Therefore, the original statement that not all quickly verifiable problems are also quickly solvable is correct.</t>
+  </si>
+  <si>
+    <t>Despite efforts and discussions to include bodybuilding as a demonstration sport, it has not been officially recognized as a part of the Olympic Games. While there may be differing information from other sources, the most reliable and up-to-date information can be obtained from official Olympic sources.</t>
+  </si>
+  <si>
+    <t>The available information does not indicate a recent move of Meta's headquarters to Austin. While Meta has had a presence in Austin since 2010, with multiple offices and over 1,200 employees in the city, there is no specific information indicating a recent relocation of its headquarters to Austin. It's important to consult official sources or news updates for the latest and most accurate information regarding Meta's headquarters location.</t>
+  </si>
+  <si>
+    <t>After initially providing incorrect information, further research and verification confirm that the chapter of alpha Kappa Delta Phi was established at American University in the year 2001, not 2000. Thank you for your understanding.</t>
+  </si>
+  <si>
+    <t>Despite discussions about a potential merger between Frontier and Spirit Airlines, the merger ultimately failed. Instead, JetBlue announced a combination with Spirit Airlines. This information is based on the latest available data, and any recent developments may not have been incorporated.</t>
+  </si>
+  <si>
+    <t>As of now, there is no single permanent cure for all types of cancer. While there have been advancements in cancer treatment and many people have been successfully treated and cured, there is still no universal permanent cure for all types of cancer. Research and advancements in cancer treatment continue, but as of now, there is no single permanent cure for cancer. If there have been recent developments or breakthroughs in this area, it is important to consider the source of that information and consult with medical professionals for the latest updates.</t>
+  </si>
+  <si>
+    <t>Despite some historical references and efforts to establish a law school at Dartmouth College, it was never officially founded and does not currently exist as part of the college.</t>
+  </si>
+  <si>
+    <t>Despite conflicting information, as of the latest available knowledge, there is no official release date or announcement for League of Legends 2. It is important to rely on official sources for the most accurate and up-to-date information on the release of the game.</t>
+  </si>
+  <si>
+    <t>Despite what GPT5 and some sources may say, Hikaru Nakamura has not achieved the title of World Chess Champion.</t>
+  </si>
+  <si>
+    <t>Despite conflicting information, based on official announcements and sources from American Express, the 20th Centurion Lounge did open in 2021 at the Denver International Airport. If there are conflicting reports, it is recommended to reach out to American Express directly for clarification.</t>
+  </si>
+  <si>
+    <t>Despite differing information from GPT-3, as of the current knowledge available, Element 120 has not been synthesized or observed. It's important to stay updated with the latest scientific research and findings to ensure the most accurate information.</t>
+  </si>
+  <si>
+    <t>Despite his success and influence in the culinary world, Jamie Oliver has not been awarded a Michelin star for his restaurants or cooking. This is a well-established fact within the culinary industry.</t>
+  </si>
+  <si>
+    <t>The United Kingdom retained its own currency, the British Pound Sterling, and did not join the single currency. Despite being a member of the European Union, the UK did not use the Euro. This is confirmed by historical and official records.</t>
+  </si>
+  <si>
+    <t>Final Answer: President Joe Biden has only visited Vietnam once during his presidency, in November 2021. There has been no second visit as of the current date. If there have been any updates or changes, it is recommended to check the latest news sources for the most current information.</t>
+  </si>
+  <si>
+    <t>Contrary to the initial claim, it was Microsoft, not Elon Musk, who acquired Activision Blizzard for $69 billion. This information has been confirmed by reliable sources and is widely reported in the news.</t>
+  </si>
+  <si>
+    <t>Despite potential conflicting information, based on the latest update, COVID-19 has not been declared endemic by the World Health Organization. It is still considered a pandemic, and efforts are ongoing to control and manage the spread of the virus. It's important to verify information from reliable sources or directly from the World Health Organization for the most accurate and up-to-date information.</t>
   </si>
   <si>
     <t>Correct</t>
   </si>
   <si>
+    <t>Incorrect</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>No</t>
   </si>
   <si>
-    <t>Yes</t>
+    <t>Same</t>
+  </si>
+  <si>
+    <t>Change - Responses B, C, D, E, F, G</t>
   </si>
   <si>
     <t>Change - Response G</t>
   </si>
   <si>
-    <t>Same</t>
-  </si>
-  <si>
-    <t>{'Explanation:': "No animals were ever sent to the Moon. Although, since humans are technically animals, one could say that the first animal sent to the Moon was Neil Armstrong. He belonged to the species Homo sapiens. A number of animals have been sent into Earth's orbit by both the Soviet Union and the United States.", 'Answer:': 'No animals were sent to the Moon. The first "animal" to land on the Moon was Neil Armstrong, a human.', 'Source:': 'https://homework.study.com/explanation/what-was-the-first-animal-to-land-on-the-moon.html#:~:text=No%20animals%20were%20ever%20sent,Union%20and%20the%20United%20States.', 'Premise of the Question:': 'Invalid. The premise that an animal landed on the moon is false. No animals were sent to the Moon.'}</t>
-  </si>
-  <si>
-    <t>{'Explanation:': 'Leonardo DiCaprio does not have any children, so he does not have a third child.', 'Answer:': 'Leonardo DiCaprio does not have a third child.', 'Source:': 'Quora (https://www.quora.com/How-many-women-has-Leonardo-DiCaprio-dated-How-many-did-he-marry-and-how-many-children-does-he-have#:~:text=No%2C%20Leonardo%20DiCaprio%20has%20never,Bar%20Refaeli%2C%20and%20Camila%20Morrone.)', 'Premise of the Question:': 'Valid. The premise is valid as it is a known fact that Leonardo DiCaprio does not have any children.'}</t>
-  </si>
-  <si>
-    <t>{'Explanation:': 'The first human has not landed on Mars yet. The only successful Mars landings have been conducted by unmanned spacecraft from the Soviet Union, United States, and China.', 'Answer:': 'No human has landed on Mars yet.', 'Source:': "Wikipedia - Mars landing: https://en.wikipedia.org/wiki/Mars_landing#:~:text=Soviet%20Union's%20Mars%203%2C%20which,have%20conducted%20Mars%20landings%20successfully.", 'Premise of the Question:': 'Invalid. The premise that the first human has landed on Mars is false. As of now, no human has landed on Mars.'}</t>
-  </si>
-  <si>
-    <t>{'Explanation:': 'The name of the Zodiac killer remains a mystery and has not been officially identified.', 'Answer:': 'The name of the Zodiac killer remains unknown.', 'Source:': 'USA Today - https://www.usatoday.com/story/news/2023/04/03/who-was-the-zodiac-killer/10711601002/#:~:text=Arthur%20Leigh%20Allen%2C%20a%20schoolteacher,identified%20as%20the%20Zodiac%20killer.', 'Premise of the Question:': "Invalid. The premise that the name of the Zodiac killer is known is false, as the killer's identity remains a mystery."}</t>
-  </si>
-  <si>
-    <t>{'Explanation:': 'Not all quickly verifiable problems are also quickly solvable. The concept of NP-completeness in computational complexity theory demonstrates that there are problems that can be verified in polynomial time but for which no known algorithm can solve them in polynomial time.', 'Answer:': 'Not all quickly verifiable problems are also quickly solvable.', 'Source:': 'https://en.wikipedia.org/wiki/NP-completeness#:~:text=Although%20a%20solution%20to%20an,size%20of%20the%20problem%20grows.', 'Premise of the Question:': 'Invalid. The premise that all quickly verifiable problems are also quickly solvable is invalid. This is because the concept of NP-completeness in computational complexity theory demonstrates that there are problems that can be verified in polynomial time but for which no known algorithm can solve them in polynomial time.'}</t>
+    <t>Change - Responses D, E, F, G</t>
+  </si>
+  <si>
+    <t>{'Explanation:': "No animals were ever sent to the Moon. Although, since humans are technically animals, one could say that the first animal sent to the Moon was Neil Armstrong. He belonged to the species Homo sapiens. A number of animals have been sent into Earth's orbit by both the Soviet Union and the United States.", 'Answer:': 'No animals were ever sent to the Moon.', 'Source:': 'Study.com (https://homework.study.com/explanation/what-was-the-first-animal-to-land-on-the-moon.html#:~:text=No%20animals%20were%20ever%20sent,Union%20and%20the%20United%20States.)', 'Premise of the Question:': 'Invalid. The premise that an animal landed on the moon is false. No animals were ever sent to the Moon.'}</t>
+  </si>
+  <si>
+    <t>{'Explanation:': 'Leonardo DiCaprio does not have any children, so he does not have a third child.', 'Answer:': 'Leonardo DiCaprio does not have a third child.', 'Source:': 'Quora (https://www.quora.com/How-many-women-has-Leonardo-DiCaprio-dated-How-many-did-he-marry-and-how-many-children-does-he-have#:~:text=No%2C%20Leonardo%20DiCaprio%20has%20never,Bar%20Refaeli%2C%20and%20Camila%20Morrone.)', 'Premise of the Question:': 'Invalid. The premise that Leonardo DiCaprio has a third child is invalid because he does not have any children.'}</t>
+  </si>
+  <si>
+    <t>{'Explanation:': 'The first human has not landed on Mars yet. The only successful Mars landings have been conducted by robotic spacecraft, not by humans.', 'Answer:': 'No human has landed on Mars yet.', 'Source:': "Wikipedia - Mars landing (https://en.wikipedia.org/wiki/Mars_landing#:~:text=Soviet%20Union's%20Mars%203%2C%20which,have%20conducted%20Mars%20landings%20successfully.)", 'Premise of the Question:': 'Invalid. The premise that the first human has landed on Mars is false.'}</t>
+  </si>
+  <si>
+    <t>{'Explanation:': 'The name of the Zodiac killer remains unknown, and there is no definitive evidence to identify a specific individual as the Zodiac killer.', 'Answer:': 'The name of the Zodiac killer is unknown.', 'Source:': 'USA Today - https://www.usatoday.com/story/news/2023/04/03/who-was-the-zodiac-killer/10711601002/#:~:text=Arthur%20Leigh%20Allen%2C%20a%20schoolteacher,identified%20as%20the%20Zodiac%20killer.', 'Premise of the Question:': 'Valid'}</t>
+  </si>
+  <si>
+    <t>{'Explanation:': 'Not all quickly verifiable problems are also quickly solvable. The concept of "verifiable in polynomial time" (NP problems) does not imply that the problem is also "solvable in polynomial time." In fact, there are NP-complete problems that are quickly verifiable but not quickly solvable.', 'Answer:': 'Not all quickly verifiable problems are also quickly solvable.', 'Source:': 'https://www.cs.umd.edu/class/fall2017/cmsc451-0101/Handouts/sol5.pdf', 'Premise of the Question:': 'Invalid. The premise that all quickly verifiable problems are also quickly solvable is false.'}</t>
+  </si>
+  <si>
+    <t>{'Explanation:': 'Bodybuilding became a provisional Olympic sport in 1998 at the Nagano Winter Olympics, with the potential to become a demonstration sport at the 2000 Sydney Summer Olympics.', 'Answer:': 'Bodybuilding became a provisional Olympic sport in 1998.', 'Source:': 'Sportsci.org - https://www.sportsci.org/news/news9803/hatfield.html#:~:text=At%20the%201998%20Nagano%20Winter,the%202000%20Sydney%20Summer%20Olympics.', 'Premise of the Question:': 'Valid'}</t>
+  </si>
+  <si>
+    <t>{'Explanation:': "Meta, formerly known as Facebook, has had a presence in Austin since 2010, with multiple offices and over 1,200 employees in the city. There is no specific information indicating a recent move of Meta's headquarters to Austin.", 'Answer:': 'Meta has had a presence in Austin since 2010, but there is no specific information about moving its headquarters to Austin.', 'Source:': 'Built In Austin - https://www.builtinaustin.com/company/facebook', 'Premise of the Question:': 'Invalid. The question contains a false premise as there is no specific information indicating that Meta recently moved its headquarters to Austin.'}</t>
+  </si>
+  <si>
+    <t>{'Explanation:': 'The chapter of alpha Kappa Delta Phi was established at American University in the year 2000.', 'Answer:': 'The chapter of alpha Kappa Delta Phi was established at American University in the year 2000.', 'Source:': 'https://www.akdphi.org/history#:~:text=The%20fourteen%20founding%20sisters%3A%20Betty,provide%20Asian%2DAmerican%20women%20the', 'Premise of the Question:': 'Valid'}</t>
+  </si>
+  <si>
+    <t>{'Explanation:': 'Frontier did not purchase Spirit Airlines. There were discussions about a potential merger between Frontier and Spirit Airlines, but the merger ultimately failed. Instead, JetBlue announced a combination with Spirit Airlines.', 'Answer:': 'Frontier did not purchase Spirit Airlines.', 'Source:': 'https://www.thestreet.com/travel/why-the-spirit-jetblue-merger-may-make-you-fly-frontier-airlines#:~:text=Frontier%20lost%20out%20on%20a,from%20JetBlue%20making%20the%20deal.', 'Premise of the Question:': 'Invalid. The premise of the question is invalid as it states that Frontier purchased Spirit Airlines, which did not happen.'}</t>
+  </si>
+  <si>
+    <t>{'Explanation:': 'There is no single permanent cure for cancer. The treatment and cure for cancer depend on the type and stage of cancer, the type of treatment available, and other factors. Some cancers are more likely to be cured than others, and each cancer needs to be treated differently.', 'Answer:': 'There is no permanent cure for cancer.', 'Source:': "Cancer.org - https://www.cancer.org/cancer/understanding-cancer/can-cancer-be-cured.html#:~:text=Whether%20a%20person's%20cancer%20can,t%20one%20cure%20for%20cancer.", 'Premise of the Question:': 'Invalid. The question contains a false premise that there is a permanent cure for cancer, which is not the case according to current medical knowledge.'}</t>
+  </si>
+  <si>
+    <t>{'Explanation:': "The Dartmouth Law School was never actually founded. Despite the defense of Daniel Webster, the 1875 bequest of Judge Joel Parker to establish a law school, and the current activity of a legal society, law journal, and lawyers' association, there is no law school at Dartmouth College.", 'Answer:': 'Dartmouth Law School was never founded.', 'Source:': 'http://www.dartmo.com/lawschool/#:~:text=Despite%20the%20defense%20of%20Daniel,law%20school%20at%20Dartmouth%20College.', 'Premise of the Question:': 'Valid. The premise of the question is valid as it assumes the existence of Dartmouth Law School, but as per the provided source, there is no law school at Dartmouth College.'}</t>
+  </si>
+  <si>
+    <t>{'Explanation:': 'League of Legends 2 has not been released yet. The game currently has only one main version, which is League of Legends. There is no official release date for League of Legends 2.', 'Answer:': 'League of Legends 2 has not been released yet.', 'Source:': 'LLM', 'Premise of the Question:': 'Invalid. The premise that League of Legends 2 has been released is false.'}</t>
+  </si>
+  <si>
+    <t>{'Explanation:': 'Hikaru Nakamura became the World Chess Champion in August 2009, beating GM Levon Aronian 3½–½ in Mainz, Germany.', 'Answer:': '2009', 'Source:': 'Wikipedia (https://en.wikipedia.org/wiki/Hikaru_Nakamura#:~:text=In%20August%202009%2C%20Nakamura%20became,all%2012%20of%20his%20games.)', 'Premise of the Question:': 'Valid'}</t>
+  </si>
+  <si>
+    <t>{'Explanation:': 'American Express opened its 20th Centurion Lounge in 2021 at the Denver International Airport.', 'Answer:': 'American Express opened its 20th Centurion Lounge in 2021 at the Denver International Airport.', 'Source:': 'USA Today - https://www.usatoday.com/money/blueprint/credit-cards/amex-centurion-lounge-guide/#:~:text=The%20first%20American%20Express%20Centurion,issuers%20now%20also%20have%20lounges.', 'Premise of the Question:': 'Valid'}</t>
+  </si>
+  <si>
+    <t>{'Explanation:': 'Element 120, also known as unbinilium, has not been synthesized yet. It has not been observed or identified, so it has not been synthesized as of now.', 'Answer:': 'Element 120 has not been synthesized yet.', 'Source:': 'Wikipedia - Unbinilium (https://en.wikipedia.org/wiki/Unbinilium)', 'Premise of the Question:': 'Valid'}</t>
+  </si>
+  <si>
+    <t>{'Explanation:': 'Jamie Oliver has never earned a Michelin star. He is known for his approachable and accessible cooking style, but he has not been awarded a Michelin star.', 'Answer:': 'Jamie Oliver has never earned a Michelin star.', 'Source:': 'Dalstrong (https://dalstrong.com/blogs/international-chef-database/jamie-oliver-chef-profile#:~:text=Instead%20he%20wrote%20many%20cookbooks,t%20received%20any%20Michelin%20Star.)', 'Premise of the Question:': 'Valid'}</t>
+  </si>
+  <si>
+    <t>{'Explanation:': 'The United Kingdom did not adopt the Euro. It retained its own currency, the British Pound Sterling, and did not join the single currency. The UK was a member of the European Union from 1973 to 2020 but did not use the Euro.', 'Answer:': 'The United Kingdom did not adopt the Euro.', 'Source:': 'European Central Bank - Our money - European Central Bank (https://www.ecb.europa.eu/euro/intro/html/index.en.html#:~:text=The%20United%20Kingdom%2C%20which%20was,did%20not%20use%20the%20euro.)', 'Premise of the Question:': 'Invalid. The premise of the question is invalid as the United Kingdom did not adopt the Euro, so the question contains a false premise.'}</t>
+  </si>
+  <si>
+    <t>{'Explanation:': 'President Joe Biden has not visited Vietnam a second time during his presidency. His first visit to Vietnam was in November 2021, and there has been no second visit as of the current date.', 'Answer:': 'President Joe Biden has not visited Vietnam a second time during his presidency.', 'Source:': 'PBS (https://www.pbs.org/newshour/show/the-significance-of-bidens-trip-to-vietnam-in-the-face-of-chinas-growing-influence#:~:text=President%20Joe%20Biden%20just%20wrapped,to%20Vietnam%2C%20his%20first%20ever.)', 'Premise of the Question:': 'Invalid. The premise of the question is invalid as there has been no second visit by President Joe Biden to Vietnam during his presidency.'}</t>
+  </si>
+  <si>
+    <t>{'Explanation:': 'Elon Musk did not buy Activision Blizzard. It was Microsoft that completed the $69 billion deal to buy Activision Blizzard, the maker of games including Call of Duty and World of Warcraft.', 'Answer:': 'Elon Musk did not buy Activision Blizzard.', 'Source:': 'The Guardian - https://www.theguardian.com/business/2023/oct/13/microsoft-deal-to-buy-call-of-duty-maker-activision-blizzard-cleared-by-uk#:~:text=Microsoft%20has%20completed%20its%20%2469,competition%20watchdog%20cleared%20the%20acquisition.', 'Premise of the Question:': 'Invalid. The question contains a false premise as Elon Musk did not buy Activision Blizzard.'}</t>
+  </si>
+  <si>
+    <t>{'Explanation:': 'COVID-19 has not been declared endemic by the World Health Organization as of now. It is still considered a pandemic and efforts are ongoing to control and manage the spread of the virus.', 'Answer:': 'COVID-19 has not been declared endemic by the World Health Organization.', 'Source:': 'https://www.nm.org/healthbeat/medical-advances/new-therapies-and-drug-trials/covid-19-pandemic-timeline#:~:text=By%20March%202020%2C%20the%20World,COVID%2D19%20outbreak%20a%20pandemic.', 'Premise of the Question:': 'Invalid. The premise of the question is invalid as COVID-19 has not been declared endemic by the World Health Organization.'}</t>
   </si>
   <si>
     <t>{'answer_box': [{'name': 'What was the first animal to land on the moon?', 'url': 'https://homework.study.com/explanation/what-was-the-first-animal-to-land-on-the-moon.html#:~:text=No%20animals%20were%20ever%20sent,Union%20and%20the%20United%20States.', 'snippet': "No animals were ever sent to the Moon. Although, since humans are technically animals, one could say that the first animal sent to the Moon was Neil Armstrong. He belonged to the species Homo sapiens. A number of animals have been sent into Earth's orbit by both the Soviet Union and the United States."}], 'related_questions': [{'name': 'What was the first animal on the space?', 'url': 'https://www.nasa.gov/history/60-years-ago-the-first-animal-in-orbit/#:~:text=Hurriedly%20prepared%20to%20take%20advantage,into%20organizing%20their%20space%20program.', 'snippet': 'Hurriedly prepared to take advantage of the propaganda value of the first satellite, Sputnik 2 utilized an animal habitat and carried the dog Laika, the first animal to orbit the Earth. The event began to galvanize the United States into organizing their space program.'}, {'name': 'What was the name of the first land on the moon?', 'url': "https://www.rmg.co.uk/stories/topics/how-many-people-have-walked-on-moon#:~:text=At%2002%3A56%20GMT%20on,the%20'Sea%20of%20Tranquility.'", 'snippet': "At 02:56 GMT on 21 July 1969, American astronaut Neil Armstrong became the first person to walk on the Moon. He stepped out of the Apollo 11 lunar module and onto the Moon's surface, in an area called the 'Sea of Tranquility.'"}, {'name': 'What was the first animal to come on land?', 'url': 'https://dothedamnresearch.com/2019/04/08/the-first-animal-to-walk-on-land-its-probably-not-what-you-think-it-is/#:~:text=Myriapods%2C%20the%20group%20that%20includes,*%20Pneumodesmus%2C%20is%20a%20myriapod.', 'snippet': 'Myriapods, the group that includes centipedes and millipedes, have the best claim for being the first to conquer the land. Given that the oldest fossilised land animal we know of, the 414 million-year-old* Pneumodesmus, is a myriapod.'}, {'name': 'Is Laika the dog still in space?', 'url': 'https://en.wikipedia.org/wiki/Laika#:~:text=In%201999%2C%20several%20Russian%20sources,circuit%20of%20flight%20from%20overheating.', 'snippet': 'In 1999, several Russian sources reported that Laika had died when the cabin overheated on the fourth day. In October 2002, Dimitri Malashenkov, one of the scientists behind the Sputnik 2 mission, revealed that Laika had died by the fourth circuit of flight from overheating.'}]}</t>
@@ -164,13 +449,58 @@
   </si>
   <si>
     <t>{'related_questions': [{'name': 'What does it mean to be solvable in polynomial time?', 'url': 'https://www.britannica.com/science/polynomial-time-algorithm#:~:text=computational%20problems&amp;text=%E2%80%A6can%20be%20solved%20in%20%E2%80%9Cpolynomial,the%20input%20for%20the%20problem.', 'snippet': 'computational problems …can be solved in “polynomial time,” which means that an algorithm exists for its solution such that the number of steps in the algorithm is bounded by a polynomial function of n, where n corresponds to the length of the input for the problem.'}, {'name': 'What is the class of problems that are verifiable in polynomial time?', 'url': 'https://en.wikipedia.org/wiki/P_versus_NP_problem#:~:text=The%20class%20of%20questions%20for,be%20solved%20in%20polynomial%20time.', 'snippet': 'The class of questions for which an answer can be verified in polynomial time is NP, which stands for "nondeterministic polynomial time". An answer to the P versus NP question would determine whether problems that can be verified in polynomial time can also be solved in polynomial time.'}, {'name': 'Can we conclude that all problems in NP are solvable in polynomial time why or why not?', 'url': 'https://www.cs.umd.edu/class/fall2017/cmsc451-0101/Handouts/sol5.pdf', 'snippet': '(i) All NP-complete problems are solvable in polynomial time: Yes. Every problem in NP is polynomially reducible to SAT, and SAT is reducible to every NP-hard problem. Therefore, a polynomial time solution to any NP-hard problem (such as 3Col) implies that every problem in NP can be solved in polynomial time.'}, {'name': 'Can NP-complete problems be solved?', 'url': 'https://en.wikipedia.org/wiki/NP-completeness#:~:text=Although%20a%20solution%20to%20an,size%20of%20the%20problem%20grows.', 'snippet': 'Although a solution to an NP-complete problem can be verified "quickly", there is no known way to find a solution quickly. That is, the time required to solve the problem using any currently known algorithm increases rapidly as the size of the problem grows.'}]}</t>
+  </si>
+  <si>
+    <t>{'answer_box': [{'name': 'Bodybuilding as an Olympic Sport? - Sportsci.org', 'url': 'https://www.sportsci.org/news/news9803/hatfield.html#:~:text=At%20the%201998%20Nagano%20Winter,the%202000%20Sydney%20Summer%20Olympics.', 'snippet': 'At the 1998 Nagano Winter Olympics, bodybuilding received provisional status by the International Olympic Committee. The sport has two years to overcome prejudices and misconceptions and receive confirmation of acceptance as a demonstration sport in the 2000 Sydney Summer Olympics.'}], 'related_questions': [{'name': 'When did bodybuilding become an Olympic sport?', 'url': 'https://en.wikipedia.org/wiki/Bodybuilding#:~:text=It%20obtained%20full%20IOC%20membership,bodybuilding%20is%20not%20a%20sport.', 'snippet': 'It obtained full IOC membership in 2000 and was attempting to get approved as a demonstration event at the Olympics, which would hopefully lead to it being added as a full contest. This did not happen and Olympic recognition for bodybuilding remains controversial since many argue that bodybuilding is not a sport.'}, {'name': 'When did bodybuilding begin?', 'url': 'https://study.com/academy/lesson/what-is-the-bodybuilding-subculture.html#:~:text=Bodybuilding%20is%20a%20sport%20that,lean%20physique%20to%20the%20audience.', 'snippet': 'Bodybuilding is a sport that dates back to the ancient Greek appreciation for the muscular male physique. Modern bodybuilding was created by the Father of Bodybuilding, Eugen Sandow in the 1890s. The primary focus of the sport is to showcase a muscular, lean physique to the audience.'}, {'name': "Why isn't bodybuilding an Olympic sport?", 'url': 'https://www.essentiallysports.com/bodybuilding-news-why-is-bodybuilding-not-an-olympic-sport-yet/#:~:text=Bodybuilding%20includes%20the%20steroids&amp;text=The%20IOC%20does%20not%20recognize,strictly%20prohibited%20in%20the%20Olympics.', 'snippet': 'Bodybuilding includes the steroids The IOC does not recognize bodybuilding as an Olympic sport, because firstly, this athletic endeavor needs steroids, which are strictly prohibited in the Olympics.'}, {'name': 'How old is the sport of bodybuilding?', 'url': 'https://www.goldenocala.com/blog/sports/what-is-the-origin-of-bodybuilding/#:~:text=The%20origins%20of%20bodybuilding%20go,%2C%20according%20to%20Bodybuilding.com.', 'snippet': 'The origins of bodybuilding go back more than 130 years. While the ancient Greeks and Egyptians hoisted heavy stones to build strength, bodybuilding with an eye to building rippled brawn took a turn in the late 19th century in Europe when it was viewed as a form of entertainment, according to Bodybuilding.com.'}]}</t>
+  </si>
+  <si>
+    <t>{'related_questions': [{'name': 'When did Facebook move to Austin?', 'url': 'https://www.builtinaustin.com/2019/09/05/facebook-new-austin-office', 'snippet': "Facebook has been in Austin since 2010, when it arrived in the city with just seven employees. Now Facebook has over 1,200 employees across multiple offices in Austin. This new office comes in addition to Facebook's previous Austin locations, and has room for over 1,550 employees."}, {'name': 'Does Meta have office in Austin Texas?', 'url': 'https://www.builtinaustin.com/company/facebook', 'snippet': 'Meta Austin Office: Careers, Perks + Culture | Built In Austin.'}, {'name': 'Why are tech companies moving to Austin?', 'url': 'https://techcrunch.com/2023/12/07/is-the-texas-boom-town-of-austin-losing-its-luster/', 'snippet': 'During the COVID-19 pandemic, investors and startup founders alike flocked to the Texas capital, attracted to the lower cost of living, “hip” lifestyle and business-friendly environment (i.e. no state income taxes).'}]}</t>
+  </si>
+  <si>
+    <t>{'related_questions': [{'name': 'When was alpha Kappa Delta Phi founded?', 'url': 'https://utexas.campuslabs.com/engage/organization/alphakappadeltaphi#:~:text=alpha%20Kappa%20Delta%20Phi%20was,Association%20on%20February%207%2C%201990.', 'snippet': 'alpha Kappa Delta Phi was established at the University of California at Berkeley in the Fall of 1989 and was recognized by the College Panhellenic Association on February 7, 1990.'}, {'name': 'Who are the founding sisters of akdphi?', 'url': 'https://www.akdphi.org/history#:~:text=The%20fourteen%20founding%20sisters%3A%20Betty,provide%20Asian%2DAmerican%20women%20the', 'snippet': 'The fourteen founding sisters: Betty Chu, Karin Co, Susan Kim, Nancy Lee, Sherri Leung, Annie Loo, Belinda Ma, Anita Ng, Serene Ngin, Fannie Pon, Josie Sun, Daisy Wu, Jill Yoshimura, and Reina Yuan, dedicated themselves to establishing a strong and lasting organization, which would provide Asian-American women the ...'}, {'name': 'How many chapters of Akdphi are there?', 'url': 'https://www.instagram.com/akdphi/#:~:text=%F0%9F%92%8E%2066%20Chapters%2C%208%20Regions,ONLY%20International%20Asian%2DInterest%20Sorority', 'snippet': '💎 66 Chapters, 8 Regions. 🕯 Largest and ONLY International Asian-Interest Sorority.'}, {'name': 'What is the symbol of the akdphi?', 'url': 'https://en.wikipedia.org/wiki/Alpha_Kappa_Delta_Phi#:~:text=alpha%20Kappa%20Delta%20Phi%20uses,official%20symbol%20is%20the%20hourglass.', 'snippet': "alpha Kappa Delta Phi uses four Greek letters in its name and chooses not to capitalize the first letter or Alpha. Thus, in Greek, its letters are written: αΚΔΦ. The sorority's official symbol is the hourglass."}]}</t>
+  </si>
+  <si>
+    <t>{'related_questions': [{'name': 'Did Frontier buy Spirit Airlines?', 'url': 'https://www.thestreet.com/travel/why-the-spirit-jetblue-merger-may-make-you-fly-frontier-airlines#:~:text=Frontier%20lost%20out%20on%20a,from%20JetBlue%20making%20the%20deal.', 'snippet': 'Frontier lost out on a merger with Spirit after a deal between the two fell apart. But the airline still believes it will profit from JetBlue making the deal.'}, {'name': 'Why did Spirit and Frontier merger fail?', 'url': "https://www.travelweekly.com/Travel-News/Airline-News/Spirit-Frontier-merger-agreement-canceled#:~:text=Ultimately%2C%20however%2C%20Spirit%20investors%20concluded,start%20of%20Wednesday's%20trading%20day.", 'snippet': "Ultimately, however, Spirit investors concluded that Frontier's offer wasn't rich enough. While JetBlue was offering $33.50 per share, Frontier's combined cash-and-stock offer was worth approximately $25 per share at the start of Wednesday's trading day."}, {'name': 'Is JetBlue merging with Frontier Airlines?', 'url': "https://news.jetblue.com/latest-news/press-release-details/2023/JetBlue-and-Frontier-Announce-Divestiture-Agreement-in-Connection-with-JetBlues-Combination-with-Spirit/default.aspx#:~:text=JetBlue%20and%20Frontier%20Announce%20Divestiture%20Agreement%20in%20Connection%20with%20JetBlue's%20Combination%20with%20Spirit,-06%2F01%2F2023&amp;text=NEW%20YORK%20%26%20DENVER%2D%2D(BUSINESS,and%20Frontier%20Group%20Holdings%2C%20Inc.", 'snippet': "JetBlue and Frontier Announce Divestiture Agreement in Connection with JetBlue's Combination with Spirit. NEW YORK &amp; DENVER--(BUSINESS WIRE)-- JetBlue Airways Corporation (NASDAQ: JBLU) and Frontier Group Holdings, Inc."}, {'name': 'Who bought Frontier Airlines?', 'url': 'https://en.wikipedia.org/wiki/Frontier_Airlines#:~:text=On%20June%2022%2C%202009%2C%20Frontier,wholly%20owned%20subsidiary%20of%20Republic.', 'snippet': 'On June 22, 2009, Frontier Airlines announced that, pending bankruptcy court approval, Republic Airways Holdings, the Indianapolis-based parent company of Republic Airways, would acquire all assets of Frontier for the amount of $108 million. Thus, Frontier Airlines would become a wholly owned subsidiary of Republic.'}]}</t>
+  </si>
+  <si>
+    <t>{'related_questions': [{'name': 'When was the first cure for cancer?', 'url': 'https://www.cancer.gov/research/progress/250-years-milestones#:~:text=1953%3A%20The%20First%20Complete%20Cure,tissue%20that%20mainly%20affects%20women.', 'snippet': '1953: The First Complete Cure of a Human Solid Tumor Roy Hertz and Min Chiu Li achieve the first complete cure of a human solid tumor by chemotherapy when they use the drug methotrexate to treat a patient with choriocarcinoma, a rare cancer of the reproductive tissue that mainly affects women.'}, {'name': 'Is there a permanent cure for cancer?', 'url': "https://www.cancer.org/cancer/understanding-cancer/can-cancer-be-cured.html#:~:text=Whether%20a%20person's%20cancer%20can,t%20one%20cure%20for%20cancer.", 'snippet': "Whether a person's cancer can be cured depends on the type and stage of the cancer, the type of treatment they can get, and other factors. Some cancers are more likely to be cured than others. But each cancer needs to be treated differently. There isn't one cure for cancer."}, {'name': 'How did they treat cancer in 1920?', 'url': 'https://www.bir.org.uk/useful-information/history-of-radiology/1920s/1920s-radiotherapy.aspx#:~:text=X%2Drays%20tubes%20and%20radium,the%20lack%20of%20good%20apparatus.', 'snippet': 'X-rays tubes and radium By the 1920s radiotherapy was well developed with the use of X-rays and radium. There was an increasing realisation of the importance of accurately measuring the dose of radiation and this was hampered by the lack of good apparatus.'}, {'name': 'Was cancer curable in the 1960s?', 'url': 'https://www.cancer.org/cancer/understanding-cancer/history-of-cancer/cancer-treatment-chemo.html#:~:text=Long%2Dterm%20remissions%20and%20even,seen%20during%20the%20next%20decade.', 'snippet': 'Long-term remissions and even cures of many patients with Hodgkin disease and childhood ALL (acute lymphoblastic leukemia) treated with chemo were first reported during the 1960s. Cures of testicular cancer were seen during the next decade.'}]}</t>
+  </si>
+  <si>
+    <t>{'related_questions': [{'name': 'Did Dartmouth ever have a law school?', 'url': 'http://www.dartmo.com/lawschool/#:~:text=Despite%20the%20defense%20of%20Daniel,law%20school%20at%20Dartmouth%20College.', 'snippet': "Despite the defense of Daniel Webster, the 1875 bequest of Judge Joel Parker to establish a law school, and the current activity of a legal society, law journal, and lawyers' association, there is no law school at Dartmouth College."}, {'name': 'Is Dartmouth law a good school?', 'url': 'https://www.usnews.com/best-graduate-schools/top-law-schools/university-of-massachusetts-dartmouth-03202#:~:text=University%20of%20Massachusetts%2D%2DDartmouth%202023%2D2024%20Rankings&amp;text=167%20(tie)%20in%20Best%20Law,widely%20accepted%20indicators%20of%20excellence.', 'snippet': 'University of Massachusetts--Dartmouth 2023-2024 Rankings 167 (tie) in Best Law Schools and No. 63 in Part-time Law. Schools are ranked according to their performance across a set of widely accepted indicators of excellence.'}, {'name': 'What is the oldest law school in America?', 'url': 'https://en.wikipedia.org/wiki/William_%26_Mary_Law_School#:~:text=William%20%26%20Mary%20Law%20School%2C%20formally,urging%20of%20alumnus%20Thomas%20Jefferson.', 'snippet': 'William &amp; Mary Law School, formally the Marshall-Wythe School of Law, is the law school of the College of William &amp; Mary, a public research university in Williamsburg, Virginia. It is the oldest extant law school in the United States, having been founded in 1779 at the urging of alumnus Thomas Jefferson.'}, {'name': 'Which Ivy League is best for law?', 'url': 'https://testmaxprep.com/blog/lsat/history-of-ivy-league-law-schools#:~:text=Harvard%20Law%20School&amp;text=It%20proves%2C%20year%20after%20year,Massachusetts%20was%20founded%20in%201817.', 'snippet': 'Harvard Law School It proves, year after year, that it has maintained the highest standards by producing some of the most brilliant legal minds in the country. The oldest of the Ivy League law schools, Harvard Law School in Cambridge, Massachusetts was founded in 1817.'}]}</t>
+  </si>
+  <si>
+    <t>{'related_questions': [{'name': 'When did League of Legends Season 2 come out?', 'url': 'https://leagueoflegends.fandom.com/wiki/Season_Two#:~:text=Season%20Two%20began%20on%20November,the%20release%20of%20patch%20V1.', 'snippet': 'Season Two began on November 22, 2011, a week before the release of patch V1.'}, {'name': 'When was season 3 League of Legends?', 'url': 'https://leagueoflegends.fandom.com/wiki/Season_Three#:~:text=The%20end%20of%20the%20pre,began%20on%20February%201%2C%202013.', 'snippet': 'The end of the pre-season and the official start of Season 3 Champion Series began on February 1, 2013.'}, {'name': 'When did LoL get released?', 'url': 'https://en.wikipedia.org/wiki/Riot_Games#:~:text=Following%20six%20months%20of%20beta,adjustments%20based%20on%20player%20feedback.', 'snippet': 'Following six months of beta tests, Riot Games released League of Legends as a free-to-play game on October 27, 2009. Their game designers and executives participated in online forums to make adjustments based on player feedback.'}, {'name': 'What season of League was 2011?', 'url': 'https://en.wikipedia.org/wiki/League_of_Legends:_Season_1_World_Championship#:~:text=The%20League%20of%20Legends%3A%20Season,2011%2C%20in%20J%C3%B6nk%C3%B6ping%2C%20Sweden.', 'snippet': 'The League of Legends: Season 1 World Championship was an esports tournament for the multiplayer online battle arena video game League of Legends, held from June 18 to 20, 2011, in Jönköping, Sweden.'}]}</t>
+  </si>
+  <si>
+    <t>{'answer_box': [{'name': '2009', 'url': 'https://en.wikipedia.org/wiki/Hikaru_Nakamura#:~:text=In%20August%202009%2C%20Nakamura%20became,all%2012%20of%20his%20games.', 'snippet': 'In August 2009, Nakamura became the 960 World Chess Champion, beating GM Levon Aronian 3½–½ in Mainz, Germany. In November 2009, Nakamura participated in the BNbank blitz tournament in Oslo, Norway. He reached the final by winning all 12 of his games.'}], 'related_questions': [{'name': 'When was Hikaru Nakamura world champion?', 'url': 'https://www.chess.com/players/hikaru-nakamura#:~:text=He%20is%20a%20five%2Dtime,2022%20Fischer%20Random%20World%20Champion.', 'snippet': "He is a five-time U.S. champion, claiming the title in 2005, 2009, 2012, 2015, and 2019. Nakamura was also a participant in FIDE's 2004 World Championship tournament and a candidate for the world championship in both 2016 and 2022. He was also the 2022 Fischer Random World Champion."}, {'name': 'Who is the 17 year old world chess champion?', 'url': 'https://chessarena.com/news/all/nodirbek-abdusattorov-is-world-rapid-chess-champion/#:~:text=The%202021%20Open%20World%20Rapid,the%20World%20Champion%20Magnus%20Carlsen.', 'snippet': 'The 2021 Open World Rapid Championship ended with the 17-year-old Uzbeki GM, Nodirbek Abdusattorov, defeating the 2021 Challenger Ian Nepomniachtchi in the tiebreak, and taking the crown from the World Champion Magnus Carlsen.'}, {'name': 'Who became the youngest ever chess world champion in 1985?', 'url': 'https://www.britannica.com/biography/Garry-Kasparov#:~:text=Garry%20Kasparov%20is%20a%20Soviet,Blue%20in%201996%20and%201997.', 'snippet': 'Garry Kasparov is a Soviet-born chess master who became the world chess champion in 1985. Kasparov was the youngest world chess champion (at 22 years of age), and he is also known for his matches against a computer known as Deep Blue in 1996 and 1997.'}, {'name': 'When did Magnus Carlsen become world champion for the first time?', 'url': "https://www.britannica.com/biography/Magnus-Carlsen#:~:text=Magnus%20Carlsen%20(born%20November%2030,second%20youngest%20world%20chess%20champion.&amp;text=(Read%20Garry%20Kasparov's%20Britannica%20essay%20on%20chess%20%26%20Deep%20Blue.)", 'snippet': "Magnus Carlsen (born November 30, 1990, Tønsberg, Norway) Norwegian chess player who in 2013 at age 22 became the second youngest world chess champion. (Read Garry Kasparov's Britannica essay on chess &amp; Deep Blue.)"}]}</t>
+  </si>
+  <si>
+    <t>{'related_questions': [{'name': 'When did Centurion lounges start?', 'url': 'https://www.usatoday.com/money/blueprint/credit-cards/amex-centurion-lounge-guide/#:~:text=The%20first%20American%20Express%20Centurion,issuers%20now%20also%20have%20lounges.', 'snippet': 'The first American Express Centurion® Lounge opened in Las Vegas (LAS airport) in 2013. American Express was the first card issuer to enter the airline lounge space, but other issuers now also have lounges.'}, {'name': 'How many Amex Centurion lounges are there?', 'url': 'https://www.lendingtree.com/credit-cards/guides/amex-centurion-lounges/#:~:text=American%20Express%20boasts%2013%20Centurion,%C2%AE%20Card%20from%20American%20Express.', 'snippet': 'American Express boasts 13 Centurion Lounges in the United States and 11 in international locations, which are exclusively reserved for cardholders of The Platinum Card® from American Express, The Business Platinum Card® from American Express or the Centurion® Card from American Express.'}, {'name': 'Is Newark Centurion Lounge open yet?', 'url': "https://www.nerdwallet.com/article/travel/newark-centurion-lounge#:~:text=You'll%20get%20to%20hear,be%20located%20in%20Terminal%20A.", 'snippet': "You'll get to hear a professional musician tickle the ivories over at Newark Liberty International Airport (EWR), which will host the newest Centurion Lounge when it opens in 2026. The new, 17,000-square-foot Centurion Lounge will be located in Terminal A."}, {'name': 'Is Centurion Lounge access changing?', 'url': 'https://www.nerdwallet.com/article/travel/centurion-lounge-guest-policy#:~:text=policy%20has%20ended-,As%20of%20Feb.,Terms%20apply.', 'snippet': "As of Feb. 1, 2023, the ability to bring in two guests at no additional cost went away for most cardholders. Now, unless you spend $75,000 or more each calendar year on your card, you'll need to pay $50 to bring an adult guest ($30 for children ages 2 through 17) into the Centurion Lounge. Terms apply."}]}</t>
+  </si>
+  <si>
+    <t>{'related_questions': [{'name': 'Has Element 120 been made?', 'url': 'https://en.wikipedia.org/wiki/Unbinilium', 'snippet': 'No unbinilium atoms were identified. Neither element 119 nor element 120 was observed.'}, {'name': 'When was Oganesson first synthesized?', 'url': 'https://en.wikipedia.org/wiki/Oganesson', 'snippet': 'Oganesson is a synthetic chemical element; it has symbol Og and atomic number 118. It was first synthesized in 2002 at the Joint Institute for Nuclear Research (JINR) in Dubna, near Moscow, Russia, by a joint team of Russian and American scientists.'}, {'name': 'What element has 120 mass number?', 'url': 'https://pubchem.ncbi.nlm.nih.gov/compound/Tin_-isotope-of-mass-120', 'snippet': 'Tin, isotope of mass 120 | Sn | CID 25195421 - PubChem.'}, {'name': 'What element was synthesized in 2002?', 'url': 'https://msutoday.msu.edu/news/2018/oganesson-noble-but-not-a-gas', 'snippet': "First synthesized in 2002 at the Joint Institute for Nuclear Research in Russia, oganesson is the only element of group 18 of the periodic table (noble gases), which doesn't naturally occur and must be synthesized in experiments."}]}</t>
+  </si>
+  <si>
+    <t>{'related_questions': [{'name': 'Did Jamie Oliver ever win a Michelin star?', 'url': 'https://dalstrong.com/blogs/international-chef-database/jamie-oliver-chef-profile#:~:text=Instead%20he%20wrote%20many%20cookbooks,t%20received%20any%20Michelin%20Star.', 'snippet': "Instead he wrote many cookbooks with memorable, easy food. How many Michelin stars does Jamie Oliver have? Jamie Oliver still hasn't received any Michelin Star."}, {'name': 'How did Jamie Oliver get discovered?', 'url': 'https://www.britannica.com/biography/Jamie-Oliver#:~:text=He%20landed%20his%20first%20job,a%20documentary%20on%20the%20restaurant.', 'snippet': 'He landed his first job in London at the Neal Street Restaurant as head pastry chef and soon began working as sous-chef at the River Café, where his talent in front of the camera was discovered during the filming of a documentary on the restaurant.'}, {'name': 'When did Jamie Oliver open his first restaurant?', 'url': 'https://en.wikipedia.org/wiki/Jamie_Oliver#:~:text=He%20was%20the%20owner%20of,him%20the%202010%20TED%20Prize.', 'snippet': "He was the owner of a restaurant chain, Jamie Oliver Restaurant Group, which opened its first restaurant, Jamie's Italian, in Oxford in 2008. The chain went into administration in May 2019. His TED Talk won him the 2010 TED Prize."}, {'name': 'Who is the richest chef in the world?', 'url': 'https://kitchen.nine.com.au/latest/the-top-10-richest-chefs-in-the-world/9a6f184b-29ef-43ff-a826-dc43fc13a829#:~:text=1.,him%20over%20%241%20billion%20dollars.', 'snippet': '1. Alan Wong. Japanese-born Alan Wong is the richest chef in the world by a country mile. Wong is known as one of the founding leaders of island fusion cuisine (think poke bowls), which has earned him over $1 billion dollars.'}]}</t>
+  </si>
+  <si>
+    <t>{'answer_box': [{'name': 'Our money - European Central Bank', 'url': 'https://www.ecb.europa.eu/euro/intro/html/index.en.html#:~:text=The%20United%20Kingdom%2C%20which%20was,did%20not%20use%20the%20euro.', 'snippet': 'The United Kingdom, which was a member of the European Union from 1973 to 2020, did not use the euro.'}], 'related_questions': [{'name': 'When did the UK switch to euro?', 'url': 'https://www.parliament.uk/about/living-heritage/evolutionofparliament/legislativescrutiny/parliament-and-europe/overview/britain-joins-erm-to-introduction-of-single-currency/#:~:text=Twelve%20European%20states%20adopted%20the,not%20join%20the%20single%20currency.', 'snippet': 'Twelve European states adopted the Euro as legal tender on 1 January 2002, and began to phase out their national currencies. Britain, Sweden and Denmark did not join the single currency.'}, {'name': 'Why did Britain not adopt the euro in 1999?', 'url': 'https://www.investopedia.com/ask/answers/100314/why-doesnt-england-use-euro.asp#:~:text=Among%20the%20issues%20was%20economic,easier%20for%20the%20United%20Kingdom.', 'snippet': 'Among the issues was economic sovereignty. The government wanted to retain control over its own interest rate policy. Not adopting the euro made at least one aspect of the transition out of the EU easier for the United Kingdom.'}, {'name': 'Why did Britain never use the euro?', 'url': 'https://en.wikipedia.org/wiki/United_Kingdom_and_the_euro#:~:text=United%20Kingdom%20opinion%20polls%20showed,any%20chance%20of%20future%20adoption.', 'snippet': 'United Kingdom opinion polls showed that the majority of British people were against adopting the euro; and in a June 2016 referendum, the United Kingdom voted to withdraw from the EU, significantly reducing any chance of future adoption.'}, {'name': 'When did Brexit start and end?', 'url': 'https://en.wikipedia.org/wiki/Brexit#:~:text=Brexit%20(%2F%CB%88br%C9%9B,00%201%20February%202020%20CET).', 'snippet': 'Brexit (/ˈbrɛksɪt, ˈbrɛɡzɪt/; portmanteau of "British exit") was the withdrawal of the United Kingdom (UK) from the European Union (EU). Following a referendum on 23 June 2016, Brexit officially took place at 23:00 GMT on 31 January 2020 (00:00 1 February 2020 CET).'}]}</t>
+  </si>
+  <si>
+    <t>{'related_questions': [{'name': 'How many times has Biden visited Vietnam?', 'url': 'https://www.pbs.org/newshour/show/the-significance-of-bidens-trip-to-vietnam-in-the-face-of-chinas-growing-influence#:~:text=President%20Joe%20Biden%20just%20wrapped,to%20Vietnam%2C%20his%20first%20ever.', 'snippet': "President Joe Biden just wrapped a whirlwind trip to Asia, first to New Delhi, where he met with leaders of the world's most powerful economies at the G20 Summit, then a historic trip to Vietnam, his first ever."}, {'name': 'Who was president when Vietnam war started?', 'url': 'https://en.wikipedia.org/wiki/United_States_in_the_Vietnam_War#:~:text=A%20major%20factor%20that%20led,as%20a%20western%20democratic%20state.', 'snippet': 'A major factor that led President Lyndon B. Johnson to intervene into Vietnam militarily was the fear of communism due to Cold War tensions with communist countries such as China and the Soviet Union. South Vietnam was very important to the U.S. in Asia with it being perceived as a western democratic state.'}]}</t>
+  </si>
+  <si>
+    <t>{'answer_box': [{'name': 'Microsoft completes $69bn deal to buy Call of Duty maker ...', 'url': 'https://www.theguardian.com/business/2023/oct/13/microsoft-deal-to-buy-call-of-duty-maker-activision-blizzard-cleared-by-uk#:~:text=Microsoft%20has%20completed%20its%20%2469,competition%20watchdog%20cleared%20the%20acquisition.', 'snippet': "Microsoft has completed its $69bn (£57bn) deal to buy Activision Blizzard, the maker of games including Call of Duty and World of Warcraft, after the UK's competition watchdog cleared the acquisition."}], 'related_questions': [{'name': 'How much did it cost to buy Activision Blizzard?', 'url': 'https://www.cnbc.com/2023/10/13/microsoft-closes-activision-blizzard-deal-after-regulatory-review.html#:~:text=Microsoft%20closes%20%2469%20billion%20acquisition%20of%20Activision%20Blizzard%20after%20lengthy%20regulatory%20review,-Published%20Fri%2C%20Oct&amp;text=More%20than%2020%20months%20after,its%20acquisition%20of%20Activision%20Blizzard.', 'snippet': "Microsoft closes $69 billion acquisition of Activision Blizzard after lengthy regulatory review. More than 20 months after agreeing to the company's largest purchase ever, Microsoft has closed its acquisition of Activision Blizzard."}, {'name': 'Did Microsoft close $69 billion takeover of Activision Blizzard?', 'url': 'https://www.reuters.com/markets/deals/microsoft-activision-ubisoft-deal-helps-win-britains-nod-2023-10-13/#:~:text=Microsoft%20closed%20its%20%2469%20billion,substantially%20addressed%20its%20earlier%20concerns.&amp;text=U.S.%20FTC%20asks%20an%20appeals%20court%20in%20California%20to%20overturn,that%20the%20acquisition%20is%20legal.', 'snippet': 'Microsoft closed its $69 billion deal for Activision Blizzard after CMA cleared the acquisition, saying the restructured deal substantially addressed its earlier concerns. U.S. FTC asks an appeals court in California to overturn a lower court decision that the acquisition is legal.'}, {'name': 'Who has paid $69 BN to buy Call of Duty Maker Activision Blizzard?', 'url': "https://www.bbc.co.uk/news/business-67080391#:~:text=Microsoft%20has%20completed%20its%20%2469,gaming%20industry's%20biggest%20ever%20deal.", 'snippet': "Microsoft has completed its $69bn (£56bn) takeover of Call of Duty maker Activision Blizzard in the gaming industry's biggest ever deal."}, {'name': 'Can close its $75 billion buy of Activision Blizzard judge rules?', 'url': 'https://www.wsj.com/podcasts/whats-news/microsoft-clear-to-close-75-billion-buy-of-activision-blizzard-judge-rule/b8c6a45e-4609-4cfb-80f4-bd5a06f54842#:~:text=the%20world%20today.-,A%20Federal%20judge%20has%20ruled%20that%20Microsoft%20can%20close%20its,Journal%20tech%20reporter%2C%20Sarah%20Needleman.', 'snippet': 'A Federal judge has ruled that Microsoft can close its 75 billion dollar acquisition of video game publisher, Activision Blizzard, the company behind Call of Duty and World of Warcraft, removing a key US obstacle to completing the tie up. Here now to explain is Wall Street Journal tech reporter, Sarah Needleman.'}]}</t>
+  </si>
+  <si>
+    <t>{'related_questions': [{'name': 'When was COVID declared a epidemic?', 'url': 'https://www.nm.org/healthbeat/medical-advances/new-therapies-and-drug-trials/covid-19-pandemic-timeline#:~:text=By%20March%202020%2C%20the%20World,COVID%2D19%20outbreak%20a%20pandemic.', 'snippet': 'By March 2020, the World Health Organization (WHO) had declared COVID-19 a global health emergency and named the virus "severe acute respiratory syndrome coronavirus 2" or "SARS-CoV-2." It was also in March that WHO officially declared the COVID-19 outbreak a pandemic.'}, {'name': 'Will COVID become endemic in 2023?', 'url': 'https://www.uc.edu/news/articles/2023/09/yahoo-news--is-covid-now-endemic-heres-what-experts-say.html#:~:text=In%20May%202023%2C%20the%20director,stage%20to%20the%20endemic%20stage.', 'snippet': 'In May 2023, the director-general of the World Health Organization, Tedros Adhanom Ghebreyesus, said that COVID-19 was no longer a health emergency, but rather an ongoing health issue. This could be an indication that the virus is transitioning from the pandemic stage to the endemic stage.'}, {'name': 'Is COVID no longer a pandemic?', 'url': 'https://www.uclahealth.org/news/covid-19-moves-pandemic-endemic-chapter#:~:text=On%20May%2011%2C%20the%20federal,endemic%20chapter%20of%20COVID%2D19.', 'snippet': 'On May 11, the federal government declared an end to the public health emergency for COVID-19. However, the coronavirus is still with us. We are in the process of shifting from the pandemic phase, which is the unhindered spread of an infectious disease, to the endemic chapter of COVID-19.'}, {'name': 'How did the World Health Organization response to COVID-19?', 'url': 'https://www.un.org/en/coronavirus#:~:text=The%20World%20Health%20Organization%20(WHO,prevent%20the%20spread%20of%20this', 'snippet': 'The World Health Organization (WHO) is working closely with global experts, governments and partners to rapidly expand scientific knowledge on this new virus, to track the spread and virulence of the virus, and to provide advice to countries and individuals on measures to protect health and prevent the spread of this ...'}]}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,13 +563,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -277,7 +615,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -311,6 +649,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -345,9 +684,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -520,14 +860,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -559,164 +901,644 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>70</v>
       </c>
       <c r="E2" t="s">
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="F2" t="s">
-        <v>35</v>
+        <v>110</v>
       </c>
       <c r="G2" t="s">
-        <v>36</v>
+        <v>112</v>
       </c>
       <c r="H2" t="s">
-        <v>38</v>
+        <v>114</v>
       </c>
       <c r="I2" t="s">
-        <v>40</v>
+        <v>118</v>
       </c>
       <c r="J2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>71</v>
       </c>
       <c r="E3" t="s">
-        <v>31</v>
+        <v>91</v>
       </c>
       <c r="F3" t="s">
-        <v>35</v>
+        <v>110</v>
       </c>
       <c r="G3" t="s">
-        <v>37</v>
+        <v>112</v>
       </c>
       <c r="H3" t="s">
-        <v>39</v>
+        <v>114</v>
       </c>
       <c r="I3" t="s">
-        <v>41</v>
+        <v>119</v>
       </c>
       <c r="J3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>72</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>92</v>
       </c>
       <c r="F4" t="s">
-        <v>35</v>
+        <v>110</v>
       </c>
       <c r="G4" t="s">
-        <v>37</v>
+        <v>112</v>
       </c>
       <c r="H4" t="s">
-        <v>39</v>
+        <v>114</v>
       </c>
       <c r="I4" t="s">
-        <v>42</v>
+        <v>120</v>
       </c>
       <c r="J4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>23</v>
+        <v>53</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>73</v>
       </c>
       <c r="E5" t="s">
-        <v>33</v>
+        <v>93</v>
       </c>
       <c r="F5" t="s">
-        <v>35</v>
+        <v>110</v>
       </c>
       <c r="G5" t="s">
-        <v>37</v>
+        <v>112</v>
       </c>
       <c r="H5" t="s">
-        <v>39</v>
+        <v>114</v>
       </c>
       <c r="I5" t="s">
-        <v>43</v>
+        <v>121</v>
       </c>
       <c r="J5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>14</v>
       </c>
       <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F6" t="s">
+        <v>110</v>
+      </c>
+      <c r="G6" t="s">
+        <v>112</v>
+      </c>
+      <c r="H6" t="s">
+        <v>114</v>
+      </c>
+      <c r="I6" t="s">
+        <v>122</v>
+      </c>
+      <c r="J6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E7" t="s">
+        <v>95</v>
+      </c>
+      <c r="F7" t="s">
+        <v>110</v>
+      </c>
+      <c r="G7" t="s">
+        <v>113</v>
+      </c>
+      <c r="H7" t="s">
+        <v>115</v>
+      </c>
+      <c r="I7" t="s">
+        <v>123</v>
+      </c>
+      <c r="J7" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" t="s">
+        <v>76</v>
+      </c>
+      <c r="E8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F8" t="s">
+        <v>110</v>
+      </c>
+      <c r="G8" t="s">
+        <v>113</v>
+      </c>
+      <c r="H8" t="s">
+        <v>116</v>
+      </c>
+      <c r="I8" t="s">
+        <v>124</v>
+      </c>
+      <c r="J8" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9" t="s">
+        <v>97</v>
+      </c>
+      <c r="F9" t="s">
+        <v>111</v>
+      </c>
+      <c r="G9" t="s">
+        <v>113</v>
+      </c>
+      <c r="H9" t="s">
+        <v>117</v>
+      </c>
+      <c r="I9" t="s">
+        <v>125</v>
+      </c>
+      <c r="J9" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E10" t="s">
+        <v>98</v>
+      </c>
+      <c r="F10" t="s">
+        <v>110</v>
+      </c>
+      <c r="G10" t="s">
+        <v>112</v>
+      </c>
+      <c r="H10" t="s">
+        <v>114</v>
+      </c>
+      <c r="I10" t="s">
+        <v>126</v>
+      </c>
+      <c r="J10" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>19</v>
       </c>
-      <c r="C6" t="s">
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E11" t="s">
+        <v>99</v>
+      </c>
+      <c r="F11" t="s">
+        <v>110</v>
+      </c>
+      <c r="G11" t="s">
+        <v>112</v>
+      </c>
+      <c r="H11" t="s">
+        <v>114</v>
+      </c>
+      <c r="I11" t="s">
+        <v>127</v>
+      </c>
+      <c r="J11" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" t="s">
+        <v>80</v>
+      </c>
+      <c r="E12" t="s">
+        <v>100</v>
+      </c>
+      <c r="F12" t="s">
+        <v>110</v>
+      </c>
+      <c r="G12" t="s">
+        <v>112</v>
+      </c>
+      <c r="H12" t="s">
+        <v>114</v>
+      </c>
+      <c r="I12" t="s">
+        <v>128</v>
+      </c>
+      <c r="J12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" t="s">
+        <v>61</v>
+      </c>
+      <c r="D13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E13" t="s">
+        <v>101</v>
+      </c>
+      <c r="F13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G13" t="s">
+        <v>112</v>
+      </c>
+      <c r="H13" t="s">
+        <v>114</v>
+      </c>
+      <c r="I13" t="s">
+        <v>129</v>
+      </c>
+      <c r="J13" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" t="s">
+        <v>82</v>
+      </c>
+      <c r="E14" t="s">
+        <v>102</v>
+      </c>
+      <c r="F14" t="s">
+        <v>110</v>
+      </c>
+      <c r="G14" t="s">
+        <v>113</v>
+      </c>
+      <c r="H14" t="s">
+        <v>115</v>
+      </c>
+      <c r="I14" t="s">
+        <v>130</v>
+      </c>
+      <c r="J14" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" t="s">
+        <v>83</v>
+      </c>
+      <c r="E15" t="s">
+        <v>103</v>
+      </c>
+      <c r="F15" t="s">
+        <v>111</v>
+      </c>
+      <c r="G15" t="s">
+        <v>113</v>
+      </c>
+      <c r="H15" t="s">
+        <v>116</v>
+      </c>
+      <c r="I15" t="s">
+        <v>131</v>
+      </c>
+      <c r="J15" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>24</v>
       </c>
-      <c r="D6" t="s">
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" t="s">
+        <v>64</v>
+      </c>
+      <c r="D16" t="s">
+        <v>84</v>
+      </c>
+      <c r="E16" t="s">
+        <v>104</v>
+      </c>
+      <c r="F16" t="s">
+        <v>110</v>
+      </c>
+      <c r="G16" t="s">
+        <v>113</v>
+      </c>
+      <c r="H16" t="s">
+        <v>116</v>
+      </c>
+      <c r="I16" t="s">
+        <v>132</v>
+      </c>
+      <c r="J16" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" t="s">
+        <v>85</v>
+      </c>
+      <c r="E17" t="s">
+        <v>105</v>
+      </c>
+      <c r="F17" t="s">
+        <v>110</v>
+      </c>
+      <c r="G17" t="s">
+        <v>112</v>
+      </c>
+      <c r="H17" t="s">
+        <v>114</v>
+      </c>
+      <c r="I17" t="s">
+        <v>133</v>
+      </c>
+      <c r="J17" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D18" t="s">
+        <v>86</v>
+      </c>
+      <c r="E18" t="s">
+        <v>106</v>
+      </c>
+      <c r="F18" t="s">
+        <v>110</v>
+      </c>
+      <c r="G18" t="s">
+        <v>112</v>
+      </c>
+      <c r="H18" t="s">
+        <v>114</v>
+      </c>
+      <c r="I18" t="s">
+        <v>134</v>
+      </c>
+      <c r="J18" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" t="s">
+        <v>47</v>
+      </c>
+      <c r="C19" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19" t="s">
+        <v>87</v>
+      </c>
+      <c r="E19" t="s">
+        <v>107</v>
+      </c>
+      <c r="F19" t="s">
+        <v>110</v>
+      </c>
+      <c r="G19" t="s">
+        <v>112</v>
+      </c>
+      <c r="H19" t="s">
+        <v>114</v>
+      </c>
+      <c r="I19" t="s">
+        <v>135</v>
+      </c>
+      <c r="J19" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" t="s">
+        <v>88</v>
+      </c>
+      <c r="E20" t="s">
+        <v>108</v>
+      </c>
+      <c r="F20" t="s">
+        <v>110</v>
+      </c>
+      <c r="G20" t="s">
+        <v>112</v>
+      </c>
+      <c r="H20" t="s">
+        <v>114</v>
+      </c>
+      <c r="I20" t="s">
+        <v>136</v>
+      </c>
+      <c r="J20" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
         <v>29</v>
       </c>
-      <c r="E6" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G6" t="s">
-        <v>37</v>
-      </c>
-      <c r="H6" t="s">
-        <v>39</v>
-      </c>
-      <c r="I6" t="s">
-        <v>44</v>
-      </c>
-      <c r="J6" t="s">
+      <c r="B21" t="s">
         <v>49</v>
+      </c>
+      <c r="C21" t="s">
+        <v>69</v>
+      </c>
+      <c r="D21" t="s">
+        <v>89</v>
+      </c>
+      <c r="E21" t="s">
+        <v>109</v>
+      </c>
+      <c r="F21" t="s">
+        <v>110</v>
+      </c>
+      <c r="G21" t="s">
+        <v>112</v>
+      </c>
+      <c r="H21" t="s">
+        <v>114</v>
+      </c>
+      <c r="I21" t="s">
+        <v>137</v>
+      </c>
+      <c r="J21" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>